<commit_message>
testdelico, testdelfund actions added temporarily
</commit_message>
<xml_diff>
--- a/vigor_ico.xlsx
+++ b/vigor_ico.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Coding\github_repos\eosio_vigor_contracts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{864755BB-5CAF-48AF-9A86-CCE8CA8582CA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3DF48D8-C18A-4A1C-8589-0B1DD7C67809}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{24ECC0CC-CB28-424B-9F73-E80DD11F83F1}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{24ECC0CC-CB28-424B-9F73-E80DD11F83F1}"/>
   </bookViews>
   <sheets>
     <sheet name="fund" sheetId="1" r:id="rId1"/>
+    <sheet name="Testing" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="64">
   <si>
     <t>disburse_qty</t>
   </si>
@@ -187,6 +188,39 @@
   </si>
   <si>
     <t>ico_type</t>
+  </si>
+  <si>
+    <t>tot_fundtype_qty</t>
+  </si>
+  <si>
+    <t>tot_disburse_qty</t>
+  </si>
+  <si>
+    <t>Table: fund
+scope: &lt;user_ac&gt;</t>
+  </si>
+  <si>
+    <t>fund_type</t>
+  </si>
+  <si>
+    <t>phase_type</t>
+  </si>
+  <si>
+    <t>current_price_pereos</t>
+  </si>
+  <si>
+    <t>proposed_price_pereos</t>
+  </si>
+  <si>
+    <t>Table: icorates
+scope: buy</t>
+  </si>
+  <si>
+    <t>Table: icorates
+scope: sell</t>
+  </si>
+  <si>
+    <t>["vigoradmin11", "vigoradmin12", "vigoradmin13", "vigoradmin14", "vigoradmin15"]</t>
   </si>
 </sst>
 </file>
@@ -216,15 +250,21 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="7">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -322,16 +362,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -349,6 +395,24 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -666,7 +730,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F214BF7-460D-491D-8FB0-F816A778561F}">
   <dimension ref="A1:L27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
@@ -832,18 +896,18 @@
     </row>
     <row r="12" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="J13" s="3" t="s">
+      <c r="J13" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="K13" s="4" t="s">
+      <c r="K13" s="3" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="J14" s="5" t="s">
+      <c r="J14" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="K14" s="6" t="s">
+      <c r="K14" s="5" t="s">
         <v>33</v>
       </c>
     </row>
@@ -851,10 +915,10 @@
       <c r="H15" t="s">
         <v>12</v>
       </c>
-      <c r="J15" s="7">
+      <c r="J15" s="6">
         <v>1598849404</v>
       </c>
-      <c r="K15" s="8">
+      <c r="K15" s="7">
         <v>1598850304</v>
       </c>
     </row>
@@ -902,10 +966,10 @@
       </c>
     </row>
     <row r="22" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B22" s="2" t="s">
+      <c r="B22" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="C22" s="2"/>
+      <c r="C22" s="8"/>
       <c r="J22" t="s">
         <v>40</v>
       </c>
@@ -966,4 +1030,230 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FEF3D99F-266B-43A4-BCC9-9488E1A5CE3E}">
+  <dimension ref="A1:L26"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="I14" sqref="I14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="9.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.88671875" customWidth="1"/>
+    <col min="8" max="8" width="17" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.5546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A1" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="B1" s="9"/>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A2" s="9"/>
+      <c r="B2" s="9"/>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="12"/>
+      <c r="B9" s="12"/>
+      <c r="C9" s="12"/>
+      <c r="D9" s="12"/>
+      <c r="E9" s="12"/>
+      <c r="F9" s="12"/>
+      <c r="G9" s="12"/>
+      <c r="H9" s="12"/>
+      <c r="I9" s="12"/>
+      <c r="J9" s="12"/>
+      <c r="K9" s="12"/>
+      <c r="L9" s="12"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A10" s="13"/>
+      <c r="B10" s="13"/>
+      <c r="C10" s="13"/>
+      <c r="D10" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="E10" s="9"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A11" s="13"/>
+      <c r="B11" s="13"/>
+      <c r="C11" s="13"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="9"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A12" s="13"/>
+      <c r="B12" s="13"/>
+      <c r="C12" s="13"/>
+      <c r="D12" s="11"/>
+      <c r="E12" s="11"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A13" s="13"/>
+      <c r="B13" s="13"/>
+      <c r="C13" s="13"/>
+      <c r="D13" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="76.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="13"/>
+      <c r="B14" s="13"/>
+      <c r="C14" s="13"/>
+      <c r="D14" t="s">
+        <v>4</v>
+      </c>
+      <c r="E14">
+        <v>40</v>
+      </c>
+      <c r="G14" s="15" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A15" s="13"/>
+      <c r="B15" s="13"/>
+      <c r="C15" s="13"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A16" s="13"/>
+      <c r="B16" s="13"/>
+      <c r="C16" s="13"/>
+    </row>
+    <row r="17" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="14"/>
+      <c r="B17" s="14"/>
+      <c r="C17" s="14"/>
+      <c r="D17" s="12"/>
+      <c r="E17" s="12"/>
+      <c r="F17" s="12"/>
+      <c r="G17" s="12"/>
+      <c r="H17" s="12"/>
+      <c r="I17" s="12"/>
+      <c r="J17" s="12"/>
+      <c r="K17" s="12"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A18" s="13"/>
+      <c r="B18" s="13"/>
+      <c r="C18" s="13"/>
+      <c r="D18" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="E18" s="9"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A19" s="13"/>
+      <c r="B19" s="13"/>
+      <c r="C19" s="13"/>
+      <c r="D19" s="9"/>
+      <c r="E19" s="9"/>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A20" s="13"/>
+      <c r="B20" s="13"/>
+      <c r="C20" s="13"/>
+      <c r="D20" s="11"/>
+      <c r="E20" s="11"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A21" s="13"/>
+      <c r="B21" s="13"/>
+      <c r="C21" s="13"/>
+      <c r="D21" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="I21" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A22" s="13"/>
+      <c r="B22" s="13"/>
+      <c r="C22" s="13"/>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A23" s="13"/>
+      <c r="B23" s="13"/>
+      <c r="C23" s="13"/>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A24" s="13"/>
+      <c r="B24" s="13"/>
+      <c r="C24" s="13"/>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A25" s="13"/>
+      <c r="B25" s="13"/>
+      <c r="C25" s="13"/>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A26" s="13"/>
+      <c r="B26" s="13"/>
+      <c r="C26" s="13"/>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A1:B2"/>
+    <mergeCell ref="D10:E11"/>
+    <mergeCell ref="D18:E19"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>